<commit_message>
Change age group ranges
</commit_message>
<xml_diff>
--- a/backend/hct_mis_api/apps/core/tests/test_files/kobo-template-invalid.xlsx
+++ b/backend/hct_mis_api/apps/core/tests/test_files/kobo-template-invalid.xlsx
@@ -5178,31 +5178,31 @@
     <t>####&lt;span style="color:black"&gt;End of questions for Individual ${individual_index}&lt;/span&gt;</t>
   </si>
   <si>
-    <t>ind_f_0_5_age_group</t>
-  </si>
-  <si>
-    <t>if((${gender_i_c}="female") and (${age}&lt;6) and (${relationship_i_c} != 'non_beneficiary'),1,0)</t>
-  </si>
-  <si>
-    <t>Check if female age 0-5 hh member</t>
-  </si>
-  <si>
-    <t>ind_f_6_11_age_group</t>
-  </si>
-  <si>
-    <t>if((${gender_i_c}="female") and (${age}&gt;5) and (${age}&lt;12) and (${relationship_i_c} != 'non_beneficiary'),1,0)</t>
-  </si>
-  <si>
-    <t>Check if female age 6-11 hh member</t>
-  </si>
-  <si>
-    <t>ind_f_12_17_age_group</t>
-  </si>
-  <si>
-    <t>if((${gender_i_c}="female") and (${age}&gt;11) and (${age}&lt;18)  and (${relationship_i_c} != 'non_beneficiary'),1,0)</t>
-  </si>
-  <si>
-    <t>Check if female age 12-17 hh member</t>
+    <t>ind_f_0_4_age_group</t>
+  </si>
+  <si>
+    <t>if((${gender_i_c}="female") and (${age}&lt;5) and (${relationship_i_c} != 'non_beneficiary'),1,0)</t>
+  </si>
+  <si>
+    <t>Check if female age 0-4 hh member</t>
+  </si>
+  <si>
+    <t>ind_f_5_12_age_group</t>
+  </si>
+  <si>
+    <t>if((${gender_i_c}="female") and (${age}&gt;4) and (${age}&lt;13) and (${relationship_i_c} != 'non_beneficiary'),1,0)</t>
+  </si>
+  <si>
+    <t>Check if female age 5-12 hh member</t>
+  </si>
+  <si>
+    <t>ind_f_13_17_age_group</t>
+  </si>
+  <si>
+    <t>if((${gender_i_c}="female") and (${age}&gt;12) and (${age}&lt;18)  and (${relationship_i_c} != 'non_beneficiary'),1,0)</t>
+  </si>
+  <si>
+    <t>Check if female age 13-17 hh member</t>
   </si>
   <si>
     <t>ind_f_18_59_age_group</t>
@@ -5256,31 +5256,31 @@
     <t>Check if pregnant hh member</t>
   </si>
   <si>
-    <t>ind_m_0_5_age_group</t>
-  </si>
-  <si>
-    <t>if((${gender_i_c}="male") and (${age}&lt;6)  and (${relationship_i_c} != 'non_beneficiary'),1,0)</t>
-  </si>
-  <si>
-    <t>Check if male age 0-5 hh member</t>
-  </si>
-  <si>
-    <t>ind_m_6_11_age_group</t>
-  </si>
-  <si>
-    <t>if((${gender_i_c}="male") and (${age}&gt;5) and (${age}&lt;12)  and (${relationship_i_c} != 'non_beneficiary'),1,0)</t>
-  </si>
-  <si>
-    <t>Check if male age 6-11 hh member</t>
-  </si>
-  <si>
-    <t>ind_m_12_17_age_group</t>
-  </si>
-  <si>
-    <t>if((${gender_i_c}="male") and (${age}&gt;11) and (${age}&lt;18)  and (${relationship_i_c} != 'non_beneficiary'),1,0)</t>
-  </si>
-  <si>
-    <t>Check if male age 12-17 hh member</t>
+    <t>ind_m_0_4_age_group</t>
+  </si>
+  <si>
+    <t>if((${gender_i_c}="male") and (${age}&lt;5)  and (${relationship_i_c} != 'non_beneficiary'),1,0)</t>
+  </si>
+  <si>
+    <t>Check if male age 0-4 hh member</t>
+  </si>
+  <si>
+    <t>ind_m_5_12_age_group</t>
+  </si>
+  <si>
+    <t>if((${gender_i_c}="male") and (${age}&gt;4) and (${age}&lt;13)  and (${relationship_i_c} != 'non_beneficiary'),1,0)</t>
+  </si>
+  <si>
+    <t>Check if male age 5-12 hh member</t>
+  </si>
+  <si>
+    <t>ind_m_13_17_age_group</t>
+  </si>
+  <si>
+    <t>if((${gender_i_c}="male") and (${age}&gt;12) and (${age}&lt;18)  and (${relationship_i_c} != 'non_beneficiary'),1,0)</t>
+  </si>
+  <si>
+    <t>Check if male age 13-17 hh member</t>
   </si>
   <si>
     <t>ind_m_18_59_age_group</t>
@@ -5301,31 +5301,31 @@
     <t>Check if male age 60+ hh member</t>
   </si>
   <si>
-    <t>ind_f_0_5_disability</t>
-  </si>
-  <si>
-    <t>if((${ind_f_0_5_age_group}=1) and (${disability_i_c}= 'disabled'),1,0)</t>
-  </si>
-  <si>
-    <t>Check if female age 0-5 hh member with disability</t>
-  </si>
-  <si>
-    <t>ind_f_6_11_disability</t>
-  </si>
-  <si>
-    <t>if((${ind_f_6_11_age_group}=1)and (${disability_i_c}= 'disabled'),1,0)</t>
-  </si>
-  <si>
-    <t>Check if females age 6-11 hh member with disability</t>
-  </si>
-  <si>
-    <t>ind_f_12_17_disability</t>
-  </si>
-  <si>
-    <t>if((${ind_f_12_17_age_group}=1) and (${disability_i_c}= 'disabled'),1,0)</t>
-  </si>
-  <si>
-    <t>Check if female age 12-17 hh member with disability</t>
+    <t>ind_f_0_4_disability</t>
+  </si>
+  <si>
+    <t>if((${ind_f_0_4_age_group}=1) and (${disability_i_c}= 'disabled'),1,0)</t>
+  </si>
+  <si>
+    <t>Check if female age 0-4 hh member with disability</t>
+  </si>
+  <si>
+    <t>ind_f_5_12_disability</t>
+  </si>
+  <si>
+    <t>if((${ind_f_5_12_age_group}=1)and (${disability_i_c}= 'disabled'),1,0)</t>
+  </si>
+  <si>
+    <t>Check if females age 5-12 hh member with disability</t>
+  </si>
+  <si>
+    <t>ind_f_13_17_disability</t>
+  </si>
+  <si>
+    <t>if((${ind_f_13_17_age_group}=1) and (${disability_i_c}= 'disabled'),1,0)</t>
+  </si>
+  <si>
+    <t>Check if female age 13-17 hh member with disability</t>
   </si>
   <si>
     <t>ind_f_18_59_disability</t>
@@ -5346,31 +5346,31 @@
     <t>Check if females Age 60+ hh member with disability</t>
   </si>
   <si>
-    <t>ind_m_0_5_disability</t>
-  </si>
-  <si>
-    <t>if((${ind_m_0_5_age_group}=1) and (${disability_i_c}= 'disabled'),1,0)</t>
-  </si>
-  <si>
-    <t>Check if males age 0-5 hh member with disability</t>
-  </si>
-  <si>
-    <t>ind_m_6_11_disability</t>
-  </si>
-  <si>
-    <t>if((${ind_m_6_11_age_group}=1) and (${disability_i_c}= 'disabled'),1,0)</t>
-  </si>
-  <si>
-    <t>Check if males age 6-11 hh member with disability</t>
-  </si>
-  <si>
-    <t>ind_m_12_17_disability</t>
-  </si>
-  <si>
-    <t>if((${ind_m_12_17_age_group}=1) and (${disability_i_c}= 'disabled'),1,0)</t>
-  </si>
-  <si>
-    <t>Check if males age 12-17 hh  member with disability</t>
+    <t>ind_m_0_4_disability</t>
+  </si>
+  <si>
+    <t>if((${ind_m_0_4_age_group}=1) and (${disability_i_c}= 'disabled'),1,0)</t>
+  </si>
+  <si>
+    <t>Check if males age 0-4 hh member with disability</t>
+  </si>
+  <si>
+    <t>ind_m_5_12_disability</t>
+  </si>
+  <si>
+    <t>if((${ind_m_5_12_age_group}=1) and (${disability_i_c}= 'disabled'),1,0)</t>
+  </si>
+  <si>
+    <t>Check if males age 5-12 hh member with disability</t>
+  </si>
+  <si>
+    <t>ind_m_13_17_disability</t>
+  </si>
+  <si>
+    <t>if((${ind_m_13_17_age_group}=1) and (${disability_i_c}= 'disabled'),1,0)</t>
+  </si>
+  <si>
+    <t>Check if males age 13-17 hh  member with disability</t>
   </si>
   <si>
     <t>ind_m_18_59_disability</t>
@@ -5445,25 +5445,25 @@
     <t>#### Composition: Females</t>
   </si>
   <si>
-    <t>f_0_5_age_group</t>
+    <t>f_0_4_age_group</t>
   </si>
   <si>
     <t>Must be 0 or more</t>
   </si>
   <si>
-    <t>Females Age 0-5</t>
-  </si>
-  <si>
-    <t>f_6_11_age_group</t>
-  </si>
-  <si>
-    <t>Females Age 6-11</t>
-  </si>
-  <si>
-    <t>f_12_17_age_group</t>
-  </si>
-  <si>
-    <t>Females Age 12-17</t>
+    <t>Females Age 0-4</t>
+  </si>
+  <si>
+    <t>f_5_12_age_group</t>
+  </si>
+  <si>
+    <t>Females Age 5-12</t>
+  </si>
+  <si>
+    <t>f_13_17_age_group</t>
+  </si>
+  <si>
+    <t>Females Age 13-17</t>
   </si>
   <si>
     <t>f_18_59_age_group</t>
@@ -5490,22 +5490,22 @@
     <t>#### Composition: Males</t>
   </si>
   <si>
-    <t>m_0_5_age_group</t>
-  </si>
-  <si>
-    <t>Males Age 0-5</t>
-  </si>
-  <si>
-    <t>m_6_11_age_group</t>
-  </si>
-  <si>
-    <t>Males  Age 6-11</t>
-  </si>
-  <si>
-    <t>m_12_17_age_group</t>
-  </si>
-  <si>
-    <t>Males Age 12-17</t>
+    <t>m_0_4_age_group</t>
+  </si>
+  <si>
+    <t>Males Age 0-4</t>
+  </si>
+  <si>
+    <t>m_5_12_age_group</t>
+  </si>
+  <si>
+    <t>Males  Age 5-12</t>
+  </si>
+  <si>
+    <t>m_13_17_age_group</t>
+  </si>
+  <si>
+    <t>Males Age 13-17</t>
   </si>
   <si>
     <t>m_18_59_age_group</t>
@@ -5520,22 +5520,22 @@
     <t>Males Age 60+</t>
   </si>
   <si>
-    <t>f_0_5_age_group_h_c</t>
-  </si>
-  <si>
-    <t xml:space="preserve">if(${collect_individual_data_h_c} = '1', sum(${ind_f_0_5_age_group}), ${f_0_5_age_group}) </t>
-  </si>
-  <si>
-    <t>f_6_11_age_group_h_c</t>
-  </si>
-  <si>
-    <t>if(${collect_individual_data_h_c} = '1', sum(${ind_f_6_11_age_group}), ${f_6_11_age_group})</t>
-  </si>
-  <si>
-    <t>f_12_17_age_group_h_c</t>
-  </si>
-  <si>
-    <t>if(${collect_individual_data_h_c} = '1', sum(${ind_f_12_17_age_group}), ${f_12_17_age_group})</t>
+    <t>f_0_4_age_group_h_c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">if(${collect_individual_data_h_c} = '1', sum(${ind_f_0_4_age_group}), ${f_0_4_age_group}) </t>
+  </si>
+  <si>
+    <t>f_5_12_age_group_h_c</t>
+  </si>
+  <si>
+    <t>if(${collect_individual_data_h_c} = '1', sum(${ind_f_5_12_age_group}), ${f_5_12_age_group})</t>
+  </si>
+  <si>
+    <t>f_13_17_age_group_h_c</t>
+  </si>
+  <si>
+    <t>if(${collect_individual_data_h_c} = '1', sum(${ind_f_13_17_age_group}), ${f_13_17_age_group})</t>
   </si>
   <si>
     <t>f_18_59_age_group_h_c</t>
@@ -5556,22 +5556,22 @@
     <t>if(${collect_individual_data_h_c} = '1', sum(${ind_pregnant}), ${pregnant})</t>
   </si>
   <si>
-    <t>m_0_5_age_group_h_c</t>
-  </si>
-  <si>
-    <t>if(${collect_individual_data_h_c} = '1', sum(${ind_m_0_5_age_group}), ${m_0_5_age_group})</t>
-  </si>
-  <si>
-    <t>m_6_11_age_group_h_c</t>
-  </si>
-  <si>
-    <t>if(${collect_individual_data_h_c} = '1', sum(${ind_m_6_11_age_group}), ${m_6_11_age_group})</t>
-  </si>
-  <si>
-    <t>m_12_17_age_group_h_c</t>
-  </si>
-  <si>
-    <t>if(${collect_individual_data_h_c} = '1', sum(${ind_m_12_17_age_group}), ${m_12_17_age_group})</t>
+    <t>m_0_4_age_group_h_c</t>
+  </si>
+  <si>
+    <t>if(${collect_individual_data_h_c} = '1', sum(${ind_m_0_4_age_group}), ${m_0_4_age_group})</t>
+  </si>
+  <si>
+    <t>m_5_12_age_group_h_c</t>
+  </si>
+  <si>
+    <t>if(${collect_individual_data_h_c} = '1', sum(${ind_m_5_12_age_group}), ${m_5_12_age_group})</t>
+  </si>
+  <si>
+    <t>m_13_17_age_group_h_c</t>
+  </si>
+  <si>
+    <t>if(${collect_individual_data_h_c} = '1', sum(${ind_m_13_17_age_group}), ${m_13_17_age_group})</t>
   </si>
   <si>
     <t>m_18_59_age_group_h_c</t>
@@ -5589,7 +5589,7 @@
     <t>hh_size_calculated</t>
   </si>
   <si>
-    <t>coalesce(${f_0_5_age_group_h_c},0)+coalesce(${f_6_11_age_group_h_c},0)+coalesce(${f_12_17_age_group_h_c},0)+coalesce(${f_18_59_age_group_h_c},0)+coalesce(${f_60_age_group_h_c},0)+coalesce(${m_0_5_age_group_h_c},0)+coalesce(${m_6_11_age_group_h_c},0)+coalesce(${m_12_17_age_group_h_c},0)+coalesce(${m_18_59_age_group_h_c},0)+coalesce(${m_60_age_group_h_c},0)</t>
+    <t>coalesce(${f_0_4_age_group_h_c},0)+coalesce(${f_5_12_age_group_h_c},0)+coalesce(${f_13_17_age_group_h_c},0)+coalesce(${f_18_59_age_group_h_c},0)+coalesce(${f_60_age_group_h_c},0)+coalesce(${m_0_4_age_group_h_c},0)+coalesce(${m_5_12_age_group_h_c},0)+coalesce(${m_13_17_age_group_h_c},0)+coalesce(${m_18_59_age_group_h_c},0)+coalesce(${m_60_age_group_h_c},0)</t>
   </si>
   <si>
     <t>Calculated composition</t>
@@ -5628,52 +5628,52 @@
     <t>#### Number of members with disability in each age group</t>
   </si>
   <si>
-    <t>f_0_5_disability</t>
-  </si>
-  <si>
-    <t>${f_0_5_age_group} &gt;0</t>
-  </si>
-  <si>
-    <t>(. &gt;= 0) and (. &lt;= ${f_0_5_age_group})</t>
+    <t>f_0_4_disability</t>
+  </si>
+  <si>
+    <t>${f_0_4_age_group} &gt;0</t>
+  </si>
+  <si>
+    <t>(. &gt;= 0) and (. &lt;= ${f_0_4_age_group})</t>
   </si>
   <si>
     <t>Can not be more than the number of members in this group</t>
   </si>
   <si>
-    <t>Females Age 0-5 with disability</t>
-  </si>
-  <si>
-    <t xml:space="preserve">out of  ${f_0_5_age_group} </t>
-  </si>
-  <si>
-    <t>f_6_11_disability</t>
-  </si>
-  <si>
-    <t>${f_6_11_age_group} &gt;0</t>
-  </si>
-  <si>
-    <t>(. &gt;= 0) and (. &lt;= ${f_6_11_age_group})</t>
-  </si>
-  <si>
-    <t>Females Age 6-11 with disability</t>
-  </si>
-  <si>
-    <t xml:space="preserve">out of  ${f_6_11_age_group} </t>
-  </si>
-  <si>
-    <t>f_12_17_disability</t>
-  </si>
-  <si>
-    <t>${f_12_17_age_group} &gt;0</t>
-  </si>
-  <si>
-    <t>(. &gt;= 0) and (. &lt;= ${f_12_17_age_group})</t>
-  </si>
-  <si>
-    <t>Females Age 12-17 with disability</t>
-  </si>
-  <si>
-    <t xml:space="preserve">out of  ${f_12_17_age_group} </t>
+    <t>Females Age 0-4 with disability</t>
+  </si>
+  <si>
+    <t xml:space="preserve">out of  ${f_0_4_age_group} </t>
+  </si>
+  <si>
+    <t>f_5_12_disability</t>
+  </si>
+  <si>
+    <t>${f_5_12_age_group} &gt;0</t>
+  </si>
+  <si>
+    <t>(. &gt;= 0) and (. &lt;= ${f_5_12_age_group})</t>
+  </si>
+  <si>
+    <t>Females Age 5-12 with disability</t>
+  </si>
+  <si>
+    <t xml:space="preserve">out of  ${f_5_12_age_group} </t>
+  </si>
+  <si>
+    <t>f_13_17_disability</t>
+  </si>
+  <si>
+    <t>${f_13_17_age_group} &gt;0</t>
+  </si>
+  <si>
+    <t>(. &gt;= 0) and (. &lt;= ${f_13_17_age_group})</t>
+  </si>
+  <si>
+    <t>Females Age 13-17 with disability</t>
+  </si>
+  <si>
+    <t xml:space="preserve">out of  ${f_13_17_age_group} </t>
   </si>
   <si>
     <t>f_18_59_disability</t>
@@ -5706,49 +5706,49 @@
     <t xml:space="preserve">out of  ${f_60_age_group} </t>
   </si>
   <si>
-    <t>m_0_5_disability</t>
-  </si>
-  <si>
-    <t>${m_0_5_age_group} &gt;0</t>
-  </si>
-  <si>
-    <t>(. &gt;= 0) and (. &lt;= ${m_0_5_age_group})</t>
-  </si>
-  <si>
-    <t>Males Age 0-5 with disability</t>
-  </si>
-  <si>
-    <t xml:space="preserve">out of  ${m_0_5_age_group} </t>
-  </si>
-  <si>
-    <t>m_6_11_disability</t>
-  </si>
-  <si>
-    <t>${m_6_11_age_group} &gt;0</t>
-  </si>
-  <si>
-    <t>(. &gt;= 0) and (. &lt;= ${m_6_11_age_group})</t>
-  </si>
-  <si>
-    <t>Males Age 6-11 with disability</t>
-  </si>
-  <si>
-    <t xml:space="preserve">out of  ${m_6_11_age_group} </t>
-  </si>
-  <si>
-    <t>m_12_17_disability</t>
-  </si>
-  <si>
-    <t>${m_12_17_age_group} &gt;0</t>
-  </si>
-  <si>
-    <t>(. &gt;= 0) and (. &lt;= ${m_12_17_age_group})</t>
-  </si>
-  <si>
-    <t>Males Age 12-17 with disability</t>
-  </si>
-  <si>
-    <t xml:space="preserve">out of  ${m_12_17_age_group} </t>
+    <t>m_0_4_disability</t>
+  </si>
+  <si>
+    <t>${m_0_4_age_group} &gt;0</t>
+  </si>
+  <si>
+    <t>(. &gt;= 0) and (. &lt;= ${m_0_4_age_group})</t>
+  </si>
+  <si>
+    <t>Males Age 0-4 with disability</t>
+  </si>
+  <si>
+    <t xml:space="preserve">out of  ${m_0_4_age_group} </t>
+  </si>
+  <si>
+    <t>m_5_12_disability</t>
+  </si>
+  <si>
+    <t>${m_5_12_age_group} &gt;0</t>
+  </si>
+  <si>
+    <t>(. &gt;= 0) and (. &lt;= ${m_5_12_age_group})</t>
+  </si>
+  <si>
+    <t>Males Age 5-12 with disability</t>
+  </si>
+  <si>
+    <t xml:space="preserve">out of  ${m_5_12_age_group} </t>
+  </si>
+  <si>
+    <t>m_13_17_disability</t>
+  </si>
+  <si>
+    <t>${m_13_17_age_group} &gt;0</t>
+  </si>
+  <si>
+    <t>(. &gt;= 0) and (. &lt;= ${m_13_17_age_group})</t>
+  </si>
+  <si>
+    <t>Males Age 13-17 with disability</t>
+  </si>
+  <si>
+    <t xml:space="preserve">out of  ${m_13_17_age_group} </t>
   </si>
   <si>
     <t>m_18_59_disability</t>
@@ -5781,40 +5781,40 @@
     <t xml:space="preserve">out of  ${m_60_age_group} </t>
   </si>
   <si>
-    <t>f_0_5_disability_h_c</t>
-  </si>
-  <si>
-    <t>if(${collect_individual_data_h_c} = '1', sum(${ind_f_0_5_disability}), ${f_0_5_disability})</t>
-  </si>
-  <si>
-    <t>Females age 0-5 with disability</t>
-  </si>
-  <si>
-    <t xml:space="preserve">out of  ${f_6_11_age_group_h_c} </t>
-  </si>
-  <si>
-    <t>f_6_11_disability_h_c</t>
-  </si>
-  <si>
-    <t>if(${collect_individual_data_h_c} = '1', sum(${ind_f_6_11_disability}), ${f_6_11_disability})</t>
-  </si>
-  <si>
-    <t>Females age 6-11 with disability</t>
-  </si>
-  <si>
-    <t xml:space="preserve">out of  ${f_0_5_age_group_h_c} </t>
-  </si>
-  <si>
-    <t>f_12_17_disability_h_c</t>
-  </si>
-  <si>
-    <t>if(${collect_individual_data_h_c} = '1', sum(${ind_f_12_17_disability}), ${f_12_17_disability})</t>
-  </si>
-  <si>
-    <t>Females age 12-17 with disability</t>
-  </si>
-  <si>
-    <t xml:space="preserve">out of  ${f_12_17_age_group_h_c} </t>
+    <t>f_0_4_disability_h_c</t>
+  </si>
+  <si>
+    <t>if(${collect_individual_data_h_c} = '1', sum(${ind_f_0_4_disability}), ${f_0_4_disability})</t>
+  </si>
+  <si>
+    <t>Females age 0-4 with disability</t>
+  </si>
+  <si>
+    <t xml:space="preserve">out of  ${f_5_12_age_group_h_c} </t>
+  </si>
+  <si>
+    <t>f_5_12_disability_h_c</t>
+  </si>
+  <si>
+    <t>if(${collect_individual_data_h_c} = '1', sum(${ind_f_5_12_disability}), ${f_5_12_disability})</t>
+  </si>
+  <si>
+    <t>Females age 5-12 with disability</t>
+  </si>
+  <si>
+    <t xml:space="preserve">out of  ${f_0_4_age_group_h_c} </t>
+  </si>
+  <si>
+    <t>f_13_17_disability_h_c</t>
+  </si>
+  <si>
+    <t>if(${collect_individual_data_h_c} = '1', sum(${ind_f_13_17_disability}), ${f_13_17_disability})</t>
+  </si>
+  <si>
+    <t>Females age 13-17 with disability</t>
+  </si>
+  <si>
+    <t xml:space="preserve">out of  ${f_13_17_age_group_h_c} </t>
   </si>
   <si>
     <t>f_18_59_disability_h_c</t>
@@ -5838,40 +5838,40 @@
     <t xml:space="preserve">out of  ${f_60_age_group_h_c} </t>
   </si>
   <si>
-    <t>m_0_5_disability_h_c</t>
-  </si>
-  <si>
-    <t>if(${collect_individual_data_h_c} = '1', sum(${ind_m_0_5_disability}), ${m_0_5_disability})</t>
-  </si>
-  <si>
-    <t>Males age 0-5 with disability</t>
-  </si>
-  <si>
-    <t xml:space="preserve">out of  ${m_6_11_age_group_h_c} </t>
-  </si>
-  <si>
-    <t>m_6_11_disability_h_c</t>
-  </si>
-  <si>
-    <t>if(${collect_individual_data_h_c} = '1', sum(${ind_m_6_11_disability}), ${m_6_11_disability})</t>
-  </si>
-  <si>
-    <t>Males age 6-11 with disability</t>
-  </si>
-  <si>
-    <t xml:space="preserve">out of  ${m_0_5_age_group_h_c} </t>
-  </si>
-  <si>
-    <t>m_12_17_disability_h_c</t>
-  </si>
-  <si>
-    <t>if(${collect_individual_data_h_c} = '1', sum(${ind_m_12_17_disability}), ${m_12_17_disability})</t>
-  </si>
-  <si>
-    <t>Males age 12-17 with disability</t>
-  </si>
-  <si>
-    <t xml:space="preserve">out of  ${m_12_17_age_group_h_c} </t>
+    <t>m_0_4_disability_h_c</t>
+  </si>
+  <si>
+    <t>if(${collect_individual_data_h_c} = '1', sum(${ind_m_0_4_disability}), ${m_0_4_disability})</t>
+  </si>
+  <si>
+    <t>Males age 0-4 with disability</t>
+  </si>
+  <si>
+    <t xml:space="preserve">out of  ${m_5_12_age_group_h_c} </t>
+  </si>
+  <si>
+    <t>m_5_12_disability_h_c</t>
+  </si>
+  <si>
+    <t>if(${collect_individual_data_h_c} = '1', sum(${ind_m_5_12_disability}), ${m_5_12_disability})</t>
+  </si>
+  <si>
+    <t>Males age 5-12 with disability</t>
+  </si>
+  <si>
+    <t xml:space="preserve">out of  ${m_0_4_age_group_h_c} </t>
+  </si>
+  <si>
+    <t>m_13_17_disability_h_c</t>
+  </si>
+  <si>
+    <t>if(${collect_individual_data_h_c} = '1', sum(${ind_m_13_17_disability}), ${m_13_17_disability})</t>
+  </si>
+  <si>
+    <t>Males age 13-17 with disability</t>
+  </si>
+  <si>
+    <t xml:space="preserve">out of  ${m_13_17_age_group_h_c} </t>
   </si>
   <si>
     <t>m_18_59_disability_h_c</t>

</xml_diff>

<commit_message>
Revert "Change age group ranges"
</commit_message>
<xml_diff>
--- a/backend/hct_mis_api/apps/core/tests/test_files/kobo-template-invalid.xlsx
+++ b/backend/hct_mis_api/apps/core/tests/test_files/kobo-template-invalid.xlsx
@@ -5178,31 +5178,31 @@
     <t>####&lt;span style="color:black"&gt;End of questions for Individual ${individual_index}&lt;/span&gt;</t>
   </si>
   <si>
-    <t>ind_f_0_4_age_group</t>
-  </si>
-  <si>
-    <t>if((${gender_i_c}="female") and (${age}&lt;5) and (${relationship_i_c} != 'non_beneficiary'),1,0)</t>
-  </si>
-  <si>
-    <t>Check if female age 0-4 hh member</t>
-  </si>
-  <si>
-    <t>ind_f_5_12_age_group</t>
-  </si>
-  <si>
-    <t>if((${gender_i_c}="female") and (${age}&gt;4) and (${age}&lt;13) and (${relationship_i_c} != 'non_beneficiary'),1,0)</t>
-  </si>
-  <si>
-    <t>Check if female age 5-12 hh member</t>
-  </si>
-  <si>
-    <t>ind_f_13_17_age_group</t>
-  </si>
-  <si>
-    <t>if((${gender_i_c}="female") and (${age}&gt;12) and (${age}&lt;18)  and (${relationship_i_c} != 'non_beneficiary'),1,0)</t>
-  </si>
-  <si>
-    <t>Check if female age 13-17 hh member</t>
+    <t>ind_f_0_5_age_group</t>
+  </si>
+  <si>
+    <t>if((${gender_i_c}="female") and (${age}&lt;6) and (${relationship_i_c} != 'non_beneficiary'),1,0)</t>
+  </si>
+  <si>
+    <t>Check if female age 0-5 hh member</t>
+  </si>
+  <si>
+    <t>ind_f_6_11_age_group</t>
+  </si>
+  <si>
+    <t>if((${gender_i_c}="female") and (${age}&gt;5) and (${age}&lt;12) and (${relationship_i_c} != 'non_beneficiary'),1,0)</t>
+  </si>
+  <si>
+    <t>Check if female age 6-11 hh member</t>
+  </si>
+  <si>
+    <t>ind_f_12_17_age_group</t>
+  </si>
+  <si>
+    <t>if((${gender_i_c}="female") and (${age}&gt;11) and (${age}&lt;18)  and (${relationship_i_c} != 'non_beneficiary'),1,0)</t>
+  </si>
+  <si>
+    <t>Check if female age 12-17 hh member</t>
   </si>
   <si>
     <t>ind_f_18_59_age_group</t>
@@ -5256,31 +5256,31 @@
     <t>Check if pregnant hh member</t>
   </si>
   <si>
-    <t>ind_m_0_4_age_group</t>
-  </si>
-  <si>
-    <t>if((${gender_i_c}="male") and (${age}&lt;5)  and (${relationship_i_c} != 'non_beneficiary'),1,0)</t>
-  </si>
-  <si>
-    <t>Check if male age 0-4 hh member</t>
-  </si>
-  <si>
-    <t>ind_m_5_12_age_group</t>
-  </si>
-  <si>
-    <t>if((${gender_i_c}="male") and (${age}&gt;4) and (${age}&lt;13)  and (${relationship_i_c} != 'non_beneficiary'),1,0)</t>
-  </si>
-  <si>
-    <t>Check if male age 5-12 hh member</t>
-  </si>
-  <si>
-    <t>ind_m_13_17_age_group</t>
-  </si>
-  <si>
-    <t>if((${gender_i_c}="male") and (${age}&gt;12) and (${age}&lt;18)  and (${relationship_i_c} != 'non_beneficiary'),1,0)</t>
-  </si>
-  <si>
-    <t>Check if male age 13-17 hh member</t>
+    <t>ind_m_0_5_age_group</t>
+  </si>
+  <si>
+    <t>if((${gender_i_c}="male") and (${age}&lt;6)  and (${relationship_i_c} != 'non_beneficiary'),1,0)</t>
+  </si>
+  <si>
+    <t>Check if male age 0-5 hh member</t>
+  </si>
+  <si>
+    <t>ind_m_6_11_age_group</t>
+  </si>
+  <si>
+    <t>if((${gender_i_c}="male") and (${age}&gt;5) and (${age}&lt;12)  and (${relationship_i_c} != 'non_beneficiary'),1,0)</t>
+  </si>
+  <si>
+    <t>Check if male age 6-11 hh member</t>
+  </si>
+  <si>
+    <t>ind_m_12_17_age_group</t>
+  </si>
+  <si>
+    <t>if((${gender_i_c}="male") and (${age}&gt;11) and (${age}&lt;18)  and (${relationship_i_c} != 'non_beneficiary'),1,0)</t>
+  </si>
+  <si>
+    <t>Check if male age 12-17 hh member</t>
   </si>
   <si>
     <t>ind_m_18_59_age_group</t>
@@ -5301,31 +5301,31 @@
     <t>Check if male age 60+ hh member</t>
   </si>
   <si>
-    <t>ind_f_0_4_disability</t>
-  </si>
-  <si>
-    <t>if((${ind_f_0_4_age_group}=1) and (${disability_i_c}= 'disabled'),1,0)</t>
-  </si>
-  <si>
-    <t>Check if female age 0-4 hh member with disability</t>
-  </si>
-  <si>
-    <t>ind_f_5_12_disability</t>
-  </si>
-  <si>
-    <t>if((${ind_f_5_12_age_group}=1)and (${disability_i_c}= 'disabled'),1,0)</t>
-  </si>
-  <si>
-    <t>Check if females age 5-12 hh member with disability</t>
-  </si>
-  <si>
-    <t>ind_f_13_17_disability</t>
-  </si>
-  <si>
-    <t>if((${ind_f_13_17_age_group}=1) and (${disability_i_c}= 'disabled'),1,0)</t>
-  </si>
-  <si>
-    <t>Check if female age 13-17 hh member with disability</t>
+    <t>ind_f_0_5_disability</t>
+  </si>
+  <si>
+    <t>if((${ind_f_0_5_age_group}=1) and (${disability_i_c}= 'disabled'),1,0)</t>
+  </si>
+  <si>
+    <t>Check if female age 0-5 hh member with disability</t>
+  </si>
+  <si>
+    <t>ind_f_6_11_disability</t>
+  </si>
+  <si>
+    <t>if((${ind_f_6_11_age_group}=1)and (${disability_i_c}= 'disabled'),1,0)</t>
+  </si>
+  <si>
+    <t>Check if females age 6-11 hh member with disability</t>
+  </si>
+  <si>
+    <t>ind_f_12_17_disability</t>
+  </si>
+  <si>
+    <t>if((${ind_f_12_17_age_group}=1) and (${disability_i_c}= 'disabled'),1,0)</t>
+  </si>
+  <si>
+    <t>Check if female age 12-17 hh member with disability</t>
   </si>
   <si>
     <t>ind_f_18_59_disability</t>
@@ -5346,31 +5346,31 @@
     <t>Check if females Age 60+ hh member with disability</t>
   </si>
   <si>
-    <t>ind_m_0_4_disability</t>
-  </si>
-  <si>
-    <t>if((${ind_m_0_4_age_group}=1) and (${disability_i_c}= 'disabled'),1,0)</t>
-  </si>
-  <si>
-    <t>Check if males age 0-4 hh member with disability</t>
-  </si>
-  <si>
-    <t>ind_m_5_12_disability</t>
-  </si>
-  <si>
-    <t>if((${ind_m_5_12_age_group}=1) and (${disability_i_c}= 'disabled'),1,0)</t>
-  </si>
-  <si>
-    <t>Check if males age 5-12 hh member with disability</t>
-  </si>
-  <si>
-    <t>ind_m_13_17_disability</t>
-  </si>
-  <si>
-    <t>if((${ind_m_13_17_age_group}=1) and (${disability_i_c}= 'disabled'),1,0)</t>
-  </si>
-  <si>
-    <t>Check if males age 13-17 hh  member with disability</t>
+    <t>ind_m_0_5_disability</t>
+  </si>
+  <si>
+    <t>if((${ind_m_0_5_age_group}=1) and (${disability_i_c}= 'disabled'),1,0)</t>
+  </si>
+  <si>
+    <t>Check if males age 0-5 hh member with disability</t>
+  </si>
+  <si>
+    <t>ind_m_6_11_disability</t>
+  </si>
+  <si>
+    <t>if((${ind_m_6_11_age_group}=1) and (${disability_i_c}= 'disabled'),1,0)</t>
+  </si>
+  <si>
+    <t>Check if males age 6-11 hh member with disability</t>
+  </si>
+  <si>
+    <t>ind_m_12_17_disability</t>
+  </si>
+  <si>
+    <t>if((${ind_m_12_17_age_group}=1) and (${disability_i_c}= 'disabled'),1,0)</t>
+  </si>
+  <si>
+    <t>Check if males age 12-17 hh  member with disability</t>
   </si>
   <si>
     <t>ind_m_18_59_disability</t>
@@ -5445,25 +5445,25 @@
     <t>#### Composition: Females</t>
   </si>
   <si>
-    <t>f_0_4_age_group</t>
+    <t>f_0_5_age_group</t>
   </si>
   <si>
     <t>Must be 0 or more</t>
   </si>
   <si>
-    <t>Females Age 0-4</t>
-  </si>
-  <si>
-    <t>f_5_12_age_group</t>
-  </si>
-  <si>
-    <t>Females Age 5-12</t>
-  </si>
-  <si>
-    <t>f_13_17_age_group</t>
-  </si>
-  <si>
-    <t>Females Age 13-17</t>
+    <t>Females Age 0-5</t>
+  </si>
+  <si>
+    <t>f_6_11_age_group</t>
+  </si>
+  <si>
+    <t>Females Age 6-11</t>
+  </si>
+  <si>
+    <t>f_12_17_age_group</t>
+  </si>
+  <si>
+    <t>Females Age 12-17</t>
   </si>
   <si>
     <t>f_18_59_age_group</t>
@@ -5490,22 +5490,22 @@
     <t>#### Composition: Males</t>
   </si>
   <si>
-    <t>m_0_4_age_group</t>
-  </si>
-  <si>
-    <t>Males Age 0-4</t>
-  </si>
-  <si>
-    <t>m_5_12_age_group</t>
-  </si>
-  <si>
-    <t>Males  Age 5-12</t>
-  </si>
-  <si>
-    <t>m_13_17_age_group</t>
-  </si>
-  <si>
-    <t>Males Age 13-17</t>
+    <t>m_0_5_age_group</t>
+  </si>
+  <si>
+    <t>Males Age 0-5</t>
+  </si>
+  <si>
+    <t>m_6_11_age_group</t>
+  </si>
+  <si>
+    <t>Males  Age 6-11</t>
+  </si>
+  <si>
+    <t>m_12_17_age_group</t>
+  </si>
+  <si>
+    <t>Males Age 12-17</t>
   </si>
   <si>
     <t>m_18_59_age_group</t>
@@ -5520,22 +5520,22 @@
     <t>Males Age 60+</t>
   </si>
   <si>
-    <t>f_0_4_age_group_h_c</t>
-  </si>
-  <si>
-    <t xml:space="preserve">if(${collect_individual_data_h_c} = '1', sum(${ind_f_0_4_age_group}), ${f_0_4_age_group}) </t>
-  </si>
-  <si>
-    <t>f_5_12_age_group_h_c</t>
-  </si>
-  <si>
-    <t>if(${collect_individual_data_h_c} = '1', sum(${ind_f_5_12_age_group}), ${f_5_12_age_group})</t>
-  </si>
-  <si>
-    <t>f_13_17_age_group_h_c</t>
-  </si>
-  <si>
-    <t>if(${collect_individual_data_h_c} = '1', sum(${ind_f_13_17_age_group}), ${f_13_17_age_group})</t>
+    <t>f_0_5_age_group_h_c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">if(${collect_individual_data_h_c} = '1', sum(${ind_f_0_5_age_group}), ${f_0_5_age_group}) </t>
+  </si>
+  <si>
+    <t>f_6_11_age_group_h_c</t>
+  </si>
+  <si>
+    <t>if(${collect_individual_data_h_c} = '1', sum(${ind_f_6_11_age_group}), ${f_6_11_age_group})</t>
+  </si>
+  <si>
+    <t>f_12_17_age_group_h_c</t>
+  </si>
+  <si>
+    <t>if(${collect_individual_data_h_c} = '1', sum(${ind_f_12_17_age_group}), ${f_12_17_age_group})</t>
   </si>
   <si>
     <t>f_18_59_age_group_h_c</t>
@@ -5556,22 +5556,22 @@
     <t>if(${collect_individual_data_h_c} = '1', sum(${ind_pregnant}), ${pregnant})</t>
   </si>
   <si>
-    <t>m_0_4_age_group_h_c</t>
-  </si>
-  <si>
-    <t>if(${collect_individual_data_h_c} = '1', sum(${ind_m_0_4_age_group}), ${m_0_4_age_group})</t>
-  </si>
-  <si>
-    <t>m_5_12_age_group_h_c</t>
-  </si>
-  <si>
-    <t>if(${collect_individual_data_h_c} = '1', sum(${ind_m_5_12_age_group}), ${m_5_12_age_group})</t>
-  </si>
-  <si>
-    <t>m_13_17_age_group_h_c</t>
-  </si>
-  <si>
-    <t>if(${collect_individual_data_h_c} = '1', sum(${ind_m_13_17_age_group}), ${m_13_17_age_group})</t>
+    <t>m_0_5_age_group_h_c</t>
+  </si>
+  <si>
+    <t>if(${collect_individual_data_h_c} = '1', sum(${ind_m_0_5_age_group}), ${m_0_5_age_group})</t>
+  </si>
+  <si>
+    <t>m_6_11_age_group_h_c</t>
+  </si>
+  <si>
+    <t>if(${collect_individual_data_h_c} = '1', sum(${ind_m_6_11_age_group}), ${m_6_11_age_group})</t>
+  </si>
+  <si>
+    <t>m_12_17_age_group_h_c</t>
+  </si>
+  <si>
+    <t>if(${collect_individual_data_h_c} = '1', sum(${ind_m_12_17_age_group}), ${m_12_17_age_group})</t>
   </si>
   <si>
     <t>m_18_59_age_group_h_c</t>
@@ -5589,7 +5589,7 @@
     <t>hh_size_calculated</t>
   </si>
   <si>
-    <t>coalesce(${f_0_4_age_group_h_c},0)+coalesce(${f_5_12_age_group_h_c},0)+coalesce(${f_13_17_age_group_h_c},0)+coalesce(${f_18_59_age_group_h_c},0)+coalesce(${f_60_age_group_h_c},0)+coalesce(${m_0_4_age_group_h_c},0)+coalesce(${m_5_12_age_group_h_c},0)+coalesce(${m_13_17_age_group_h_c},0)+coalesce(${m_18_59_age_group_h_c},0)+coalesce(${m_60_age_group_h_c},0)</t>
+    <t>coalesce(${f_0_5_age_group_h_c},0)+coalesce(${f_6_11_age_group_h_c},0)+coalesce(${f_12_17_age_group_h_c},0)+coalesce(${f_18_59_age_group_h_c},0)+coalesce(${f_60_age_group_h_c},0)+coalesce(${m_0_5_age_group_h_c},0)+coalesce(${m_6_11_age_group_h_c},0)+coalesce(${m_12_17_age_group_h_c},0)+coalesce(${m_18_59_age_group_h_c},0)+coalesce(${m_60_age_group_h_c},0)</t>
   </si>
   <si>
     <t>Calculated composition</t>
@@ -5628,52 +5628,52 @@
     <t>#### Number of members with disability in each age group</t>
   </si>
   <si>
-    <t>f_0_4_disability</t>
-  </si>
-  <si>
-    <t>${f_0_4_age_group} &gt;0</t>
-  </si>
-  <si>
-    <t>(. &gt;= 0) and (. &lt;= ${f_0_4_age_group})</t>
+    <t>f_0_5_disability</t>
+  </si>
+  <si>
+    <t>${f_0_5_age_group} &gt;0</t>
+  </si>
+  <si>
+    <t>(. &gt;= 0) and (. &lt;= ${f_0_5_age_group})</t>
   </si>
   <si>
     <t>Can not be more than the number of members in this group</t>
   </si>
   <si>
-    <t>Females Age 0-4 with disability</t>
-  </si>
-  <si>
-    <t xml:space="preserve">out of  ${f_0_4_age_group} </t>
-  </si>
-  <si>
-    <t>f_5_12_disability</t>
-  </si>
-  <si>
-    <t>${f_5_12_age_group} &gt;0</t>
-  </si>
-  <si>
-    <t>(. &gt;= 0) and (. &lt;= ${f_5_12_age_group})</t>
-  </si>
-  <si>
-    <t>Females Age 5-12 with disability</t>
-  </si>
-  <si>
-    <t xml:space="preserve">out of  ${f_5_12_age_group} </t>
-  </si>
-  <si>
-    <t>f_13_17_disability</t>
-  </si>
-  <si>
-    <t>${f_13_17_age_group} &gt;0</t>
-  </si>
-  <si>
-    <t>(. &gt;= 0) and (. &lt;= ${f_13_17_age_group})</t>
-  </si>
-  <si>
-    <t>Females Age 13-17 with disability</t>
-  </si>
-  <si>
-    <t xml:space="preserve">out of  ${f_13_17_age_group} </t>
+    <t>Females Age 0-5 with disability</t>
+  </si>
+  <si>
+    <t xml:space="preserve">out of  ${f_0_5_age_group} </t>
+  </si>
+  <si>
+    <t>f_6_11_disability</t>
+  </si>
+  <si>
+    <t>${f_6_11_age_group} &gt;0</t>
+  </si>
+  <si>
+    <t>(. &gt;= 0) and (. &lt;= ${f_6_11_age_group})</t>
+  </si>
+  <si>
+    <t>Females Age 6-11 with disability</t>
+  </si>
+  <si>
+    <t xml:space="preserve">out of  ${f_6_11_age_group} </t>
+  </si>
+  <si>
+    <t>f_12_17_disability</t>
+  </si>
+  <si>
+    <t>${f_12_17_age_group} &gt;0</t>
+  </si>
+  <si>
+    <t>(. &gt;= 0) and (. &lt;= ${f_12_17_age_group})</t>
+  </si>
+  <si>
+    <t>Females Age 12-17 with disability</t>
+  </si>
+  <si>
+    <t xml:space="preserve">out of  ${f_12_17_age_group} </t>
   </si>
   <si>
     <t>f_18_59_disability</t>
@@ -5706,49 +5706,49 @@
     <t xml:space="preserve">out of  ${f_60_age_group} </t>
   </si>
   <si>
-    <t>m_0_4_disability</t>
-  </si>
-  <si>
-    <t>${m_0_4_age_group} &gt;0</t>
-  </si>
-  <si>
-    <t>(. &gt;= 0) and (. &lt;= ${m_0_4_age_group})</t>
-  </si>
-  <si>
-    <t>Males Age 0-4 with disability</t>
-  </si>
-  <si>
-    <t xml:space="preserve">out of  ${m_0_4_age_group} </t>
-  </si>
-  <si>
-    <t>m_5_12_disability</t>
-  </si>
-  <si>
-    <t>${m_5_12_age_group} &gt;0</t>
-  </si>
-  <si>
-    <t>(. &gt;= 0) and (. &lt;= ${m_5_12_age_group})</t>
-  </si>
-  <si>
-    <t>Males Age 5-12 with disability</t>
-  </si>
-  <si>
-    <t xml:space="preserve">out of  ${m_5_12_age_group} </t>
-  </si>
-  <si>
-    <t>m_13_17_disability</t>
-  </si>
-  <si>
-    <t>${m_13_17_age_group} &gt;0</t>
-  </si>
-  <si>
-    <t>(. &gt;= 0) and (. &lt;= ${m_13_17_age_group})</t>
-  </si>
-  <si>
-    <t>Males Age 13-17 with disability</t>
-  </si>
-  <si>
-    <t xml:space="preserve">out of  ${m_13_17_age_group} </t>
+    <t>m_0_5_disability</t>
+  </si>
+  <si>
+    <t>${m_0_5_age_group} &gt;0</t>
+  </si>
+  <si>
+    <t>(. &gt;= 0) and (. &lt;= ${m_0_5_age_group})</t>
+  </si>
+  <si>
+    <t>Males Age 0-5 with disability</t>
+  </si>
+  <si>
+    <t xml:space="preserve">out of  ${m_0_5_age_group} </t>
+  </si>
+  <si>
+    <t>m_6_11_disability</t>
+  </si>
+  <si>
+    <t>${m_6_11_age_group} &gt;0</t>
+  </si>
+  <si>
+    <t>(. &gt;= 0) and (. &lt;= ${m_6_11_age_group})</t>
+  </si>
+  <si>
+    <t>Males Age 6-11 with disability</t>
+  </si>
+  <si>
+    <t xml:space="preserve">out of  ${m_6_11_age_group} </t>
+  </si>
+  <si>
+    <t>m_12_17_disability</t>
+  </si>
+  <si>
+    <t>${m_12_17_age_group} &gt;0</t>
+  </si>
+  <si>
+    <t>(. &gt;= 0) and (. &lt;= ${m_12_17_age_group})</t>
+  </si>
+  <si>
+    <t>Males Age 12-17 with disability</t>
+  </si>
+  <si>
+    <t xml:space="preserve">out of  ${m_12_17_age_group} </t>
   </si>
   <si>
     <t>m_18_59_disability</t>
@@ -5781,40 +5781,40 @@
     <t xml:space="preserve">out of  ${m_60_age_group} </t>
   </si>
   <si>
-    <t>f_0_4_disability_h_c</t>
-  </si>
-  <si>
-    <t>if(${collect_individual_data_h_c} = '1', sum(${ind_f_0_4_disability}), ${f_0_4_disability})</t>
-  </si>
-  <si>
-    <t>Females age 0-4 with disability</t>
-  </si>
-  <si>
-    <t xml:space="preserve">out of  ${f_5_12_age_group_h_c} </t>
-  </si>
-  <si>
-    <t>f_5_12_disability_h_c</t>
-  </si>
-  <si>
-    <t>if(${collect_individual_data_h_c} = '1', sum(${ind_f_5_12_disability}), ${f_5_12_disability})</t>
-  </si>
-  <si>
-    <t>Females age 5-12 with disability</t>
-  </si>
-  <si>
-    <t xml:space="preserve">out of  ${f_0_4_age_group_h_c} </t>
-  </si>
-  <si>
-    <t>f_13_17_disability_h_c</t>
-  </si>
-  <si>
-    <t>if(${collect_individual_data_h_c} = '1', sum(${ind_f_13_17_disability}), ${f_13_17_disability})</t>
-  </si>
-  <si>
-    <t>Females age 13-17 with disability</t>
-  </si>
-  <si>
-    <t xml:space="preserve">out of  ${f_13_17_age_group_h_c} </t>
+    <t>f_0_5_disability_h_c</t>
+  </si>
+  <si>
+    <t>if(${collect_individual_data_h_c} = '1', sum(${ind_f_0_5_disability}), ${f_0_5_disability})</t>
+  </si>
+  <si>
+    <t>Females age 0-5 with disability</t>
+  </si>
+  <si>
+    <t xml:space="preserve">out of  ${f_6_11_age_group_h_c} </t>
+  </si>
+  <si>
+    <t>f_6_11_disability_h_c</t>
+  </si>
+  <si>
+    <t>if(${collect_individual_data_h_c} = '1', sum(${ind_f_6_11_disability}), ${f_6_11_disability})</t>
+  </si>
+  <si>
+    <t>Females age 6-11 with disability</t>
+  </si>
+  <si>
+    <t xml:space="preserve">out of  ${f_0_5_age_group_h_c} </t>
+  </si>
+  <si>
+    <t>f_12_17_disability_h_c</t>
+  </si>
+  <si>
+    <t>if(${collect_individual_data_h_c} = '1', sum(${ind_f_12_17_disability}), ${f_12_17_disability})</t>
+  </si>
+  <si>
+    <t>Females age 12-17 with disability</t>
+  </si>
+  <si>
+    <t xml:space="preserve">out of  ${f_12_17_age_group_h_c} </t>
   </si>
   <si>
     <t>f_18_59_disability_h_c</t>
@@ -5838,40 +5838,40 @@
     <t xml:space="preserve">out of  ${f_60_age_group_h_c} </t>
   </si>
   <si>
-    <t>m_0_4_disability_h_c</t>
-  </si>
-  <si>
-    <t>if(${collect_individual_data_h_c} = '1', sum(${ind_m_0_4_disability}), ${m_0_4_disability})</t>
-  </si>
-  <si>
-    <t>Males age 0-4 with disability</t>
-  </si>
-  <si>
-    <t xml:space="preserve">out of  ${m_5_12_age_group_h_c} </t>
-  </si>
-  <si>
-    <t>m_5_12_disability_h_c</t>
-  </si>
-  <si>
-    <t>if(${collect_individual_data_h_c} = '1', sum(${ind_m_5_12_disability}), ${m_5_12_disability})</t>
-  </si>
-  <si>
-    <t>Males age 5-12 with disability</t>
-  </si>
-  <si>
-    <t xml:space="preserve">out of  ${m_0_4_age_group_h_c} </t>
-  </si>
-  <si>
-    <t>m_13_17_disability_h_c</t>
-  </si>
-  <si>
-    <t>if(${collect_individual_data_h_c} = '1', sum(${ind_m_13_17_disability}), ${m_13_17_disability})</t>
-  </si>
-  <si>
-    <t>Males age 13-17 with disability</t>
-  </si>
-  <si>
-    <t xml:space="preserve">out of  ${m_13_17_age_group_h_c} </t>
+    <t>m_0_5_disability_h_c</t>
+  </si>
+  <si>
+    <t>if(${collect_individual_data_h_c} = '1', sum(${ind_m_0_5_disability}), ${m_0_5_disability})</t>
+  </si>
+  <si>
+    <t>Males age 0-5 with disability</t>
+  </si>
+  <si>
+    <t xml:space="preserve">out of  ${m_6_11_age_group_h_c} </t>
+  </si>
+  <si>
+    <t>m_6_11_disability_h_c</t>
+  </si>
+  <si>
+    <t>if(${collect_individual_data_h_c} = '1', sum(${ind_m_6_11_disability}), ${m_6_11_disability})</t>
+  </si>
+  <si>
+    <t>Males age 6-11 with disability</t>
+  </si>
+  <si>
+    <t xml:space="preserve">out of  ${m_0_5_age_group_h_c} </t>
+  </si>
+  <si>
+    <t>m_12_17_disability_h_c</t>
+  </si>
+  <si>
+    <t>if(${collect_individual_data_h_c} = '1', sum(${ind_m_12_17_disability}), ${m_12_17_disability})</t>
+  </si>
+  <si>
+    <t>Males age 12-17 with disability</t>
+  </si>
+  <si>
+    <t xml:space="preserve">out of  ${m_12_17_age_group_h_c} </t>
   </si>
   <si>
     <t>m_18_59_disability_h_c</t>

</xml_diff>